<commit_message>
last days working hours
</commit_message>
<xml_diff>
--- a/Documentation/rock-the-net-working-hours-bergler-bobek-janeczek-mair-oezsoy.xlsx
+++ b/Documentation/rock-the-net-working-hours-bergler-bobek-janeczek-mair-oezsoy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bobek" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>PHASE</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Mibble is one son of a API</t>
+  </si>
+  <si>
+    <t>Reading out of the "NETSCREEN-SMI.mib" and "NS-POLICY.mib" files</t>
+  </si>
+  <si>
+    <t>Reading wasn't the problem. I had some issues with Eclipse adding the newly created mib/ directory to the Build-Path</t>
+  </si>
+  <si>
+    <t>Reading out of Mib-Files</t>
   </si>
 </sst>
 </file>
@@ -258,9 +267,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -280,50 +286,53 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -715,14 +724,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
@@ -733,106 +742,106 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>41900</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="E5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="16">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="14">
         <f>SUM(E5:E11)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="14">
         <f>SUM(F5:F11)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -861,14 +870,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
@@ -879,106 +888,106 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>41900</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="E5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="14">
         <f>SUM(E5:E11)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="14">
         <f>SUM(F5:F11)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -994,7 +1003,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,8 +1011,8 @@
     <col min="2" max="2" width="10.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" style="6" customWidth="1"/>
     <col min="4" max="4" width="35.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12" style="29" customWidth="1"/>
-    <col min="6" max="6" width="9" style="29" customWidth="1"/>
+    <col min="5" max="5" width="12" style="26" customWidth="1"/>
+    <col min="6" max="6" width="9" style="26" customWidth="1"/>
     <col min="7" max="7" width="49.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1012,218 +1021,230 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:7" s="6" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>41900</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="E5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>41892</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <v>0.125</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>41907</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>0.125</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="18">
         <v>0.27083333333333331</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>41939</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>0.14583333333333334</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>41940</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>0.125</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="18">
         <v>0.14097222222222222</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="8">
+        <v>41941</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="19">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="14">
         <f>SUM(E5:E11)</f>
-        <v>0.5625</v>
-      </c>
-      <c r="F12" s="16">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F12" s="14">
         <f>SUM(F5:F11)</f>
-        <v>0.66180555555555554</v>
-      </c>
-      <c r="G12" s="17"/>
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1239,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,7 +1269,8 @@
     <col min="2" max="2" width="10.109375"/>
     <col min="3" max="3" width="15.5546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" style="6"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="26"/>
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1257,176 +1279,186 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>41900</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="E5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>41939</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <v>0.20833333333333334</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>41940</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="18">
         <v>0.14097222222222222</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="8">
+        <v>41941</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="19">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="14">
         <f>SUM(E5:E9)</f>
-        <v>0.39583333333333337</v>
-      </c>
-      <c r="F10" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F10" s="14">
         <f>SUM(F5:F9)</f>
-        <v>0.32847222222222222</v>
-      </c>
-      <c r="G10" s="17"/>
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1434,7 +1466,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1457,14 +1489,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
@@ -1474,90 +1506,90 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>41900</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="E5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="14">
         <f>SUM(E5:E9)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <f>SUM(F5:F9)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1572,7 +1604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1584,104 +1616,104 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <f>SumEstBergler</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <f>SumActBergler</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <f>SumEstBobek</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="22">
         <f>SumActBobek</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <f>SumEstJaneczek</f>
-        <v>0.5625</v>
-      </c>
-      <c r="D8" s="21">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D8" s="19">
         <f>SumActJaneczek</f>
-        <v>0.66180555555555554</v>
+        <v>0.76041666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="18">
         <f>SumEstMair</f>
-        <v>0.39583333333333337</v>
-      </c>
-      <c r="D9" s="21">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D9" s="19">
         <f>SumActMair</f>
-        <v>0.32847222222222222</v>
+        <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="18">
         <f>SumEstOezsoy</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="19">
         <f>SumActOezsoy</f>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="18">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="D11" s="21">
+        <v>1.125</v>
+      </c>
+      <c r="D11" s="19">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>0.99027777777777781</v>
+        <v>1.1875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All Up to date
</commit_message>
<xml_diff>
--- a/Documentation/rock-the-net-working-hours-bergler-bobek-janeczek-mair-oezsoy.xlsx
+++ b/Documentation/rock-the-net-working-hours-bergler-bobek-janeczek-mair-oezsoy.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Bobek" sheetId="1" r:id="rId1"/>
@@ -16,22 +16,22 @@
   </sheets>
   <definedNames>
     <definedName name="SumActBergler">Bergler!$F$14</definedName>
-    <definedName name="SumActBobek">Bobek!$F$12</definedName>
+    <definedName name="SumActBobek">Bobek!$F$16</definedName>
     <definedName name="SumActJaneczek">Janeczek!$F$13</definedName>
     <definedName name="SumActMair">Mair!$F$13</definedName>
     <definedName name="SumActOezsoy">Oezsoy!$F$10</definedName>
     <definedName name="SumEstBergler">Bergler!$E$14</definedName>
-    <definedName name="SumEstBobek">Bobek!$E$12</definedName>
+    <definedName name="SumEstBobek">Bobek!$E$16</definedName>
     <definedName name="SumEstJaneczek">Janeczek!$E$13</definedName>
     <definedName name="SumEstMair">Mair!$E$13</definedName>
     <definedName name="SumEstOezsoy">Oezsoy!$E$10</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="89">
   <si>
     <t>Working Hours</t>
   </si>
@@ -268,16 +268,46 @@
   </si>
   <si>
     <t>The downloads took more time than estimated</t>
+  </si>
+  <si>
+    <t>User-Stories</t>
+  </si>
+  <si>
+    <t>GUI - Erste Konzepte</t>
+  </si>
+  <si>
+    <t>Design, Recherche</t>
+  </si>
+  <si>
+    <t>GUI-Mockups; JavaFX: Recherche, Pros/Cons;</t>
+  </si>
+  <si>
+    <t>10.16.2014</t>
+  </si>
+  <si>
+    <t>GUI-Erstellung(Pop-ups)</t>
+  </si>
+  <si>
+    <t>10.26.2014</t>
+  </si>
+  <si>
+    <t>Recherche nach geeigneten GUI-Testing-Tool</t>
+  </si>
+  <si>
+    <t>10.30.2014</t>
+  </si>
+  <si>
+    <t>Tabelle befüllen mit Daten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,7 +434,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -427,6 +457,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -434,132 +501,144 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="6" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="7" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="6" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="7" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="6" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="7" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="6" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="7" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,7 +727,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -722,7 +801,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -757,7 +835,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -933,156 +1010,280 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="B1:G12"/>
+  <dimension ref="B1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="8.85546875" style="4"/>
-    <col min="4" max="4" width="23" style="4"/>
-    <col min="5" max="5" width="12.85546875" style="4"/>
-    <col min="6" max="6" width="9.7109375" style="4"/>
+    <col min="2" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="23" style="1"/>
+    <col min="5" max="5" width="12.85546875" style="1"/>
+    <col min="6" max="6" width="9.7109375" style="1"/>
     <col min="7" max="7" width="52.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:7" ht="18.75" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="2:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:7" ht="16.149999999999999" customHeight="1">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
-        <v>41900</v>
-      </c>
-      <c r="C5" s="9" t="s">
+    <row r="5" spans="2:7" ht="15" customHeight="1">
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15" customHeight="1">
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10">
-        <v>2.0833333333333301E-2</v>
-      </c>
-      <c r="F5" s="10">
-        <v>2.0833333333333301E-2</v>
-      </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="E6" s="43">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F6" s="43">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" customHeight="1">
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="43">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F7" s="43">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="43">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F8" s="43">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" ht="15" customHeight="1">
+      <c r="B9" s="5">
+        <v>41680</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="43">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F9" s="43">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7" ht="15" customHeight="1">
+      <c r="B10" s="5">
+        <v>41921</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="43">
+        <v>0.125</v>
+      </c>
+      <c r="F10" s="43">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7" ht="15" customHeight="1">
+      <c r="B11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7" ht="15" customHeight="1">
+      <c r="B12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" customHeight="1">
+      <c r="B13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" ht="15" customHeight="1">
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.1875</v>
+      </c>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:7" ht="15" customHeight="1">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="2:7" ht="15" customHeight="1">
+      <c r="B16" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="15">
+      <c r="C16" s="45"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="12">
         <f>SUM(E5:E11)</f>
-        <v>2.0833333333333301E-2</v>
-      </c>
-      <c r="F12" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F16" s="12">
         <f>SUM(F5:F11)</f>
-        <v>2.0833333333333301E-2</v>
-      </c>
-      <c r="G12" s="14"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1090,252 +1291,252 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="B1:G14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" style="4"/>
-    <col min="3" max="3" width="15.7109375" style="4"/>
-    <col min="4" max="4" width="23" style="4"/>
-    <col min="5" max="5" width="12.85546875" style="4"/>
-    <col min="6" max="6" width="9.7109375" style="4"/>
+    <col min="2" max="2" width="10.42578125" style="1"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="4" max="4" width="23" style="1"/>
+    <col min="5" max="5" width="12.85546875" style="1"/>
+    <col min="6" max="6" width="9.7109375" style="1"/>
     <col min="7" max="7" width="52.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:7" ht="18.75" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+    <row r="5" spans="2:7">
+      <c r="B5" s="5">
         <v>41900</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>2.0844907407407399E-2</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="2:7" ht="30">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <v>0.105115740740741</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" ht="45">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>8.3182870370370393E-2</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" ht="45">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <v>8.3321759259259304E-2</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>4.1678240740740703E-2</v>
       </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>0.125</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="15">
         <v>0.16666666666666699</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="2:7" ht="75">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="14">
         <v>0.125</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <v>0.125</v>
       </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7" ht="45">
+      <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="14">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7" ht="30">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="16">
         <v>0.125</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="16">
         <v>0.125</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:7" ht="15" customHeight="1">
+      <c r="B14" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="15">
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="12">
         <f>SUM(E5:E13)</f>
         <v>0.77083333333333315</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <f>SUM(F5:F13)</f>
         <v>0.83414351851851909</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1348,256 +1549,256 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.140625" style="4"/>
-    <col min="3" max="3" width="15.7109375" style="4"/>
-    <col min="4" max="4" width="48.7109375" style="4"/>
-    <col min="5" max="5" width="12" style="20"/>
-    <col min="6" max="6" width="9" style="20"/>
-    <col min="7" max="7" width="49.7109375" style="6"/>
+    <col min="2" max="2" width="10.140625" style="1"/>
+    <col min="3" max="3" width="15.7109375" style="1"/>
+    <col min="4" max="4" width="48.7109375" style="1"/>
+    <col min="5" max="5" width="12" style="17"/>
+    <col min="6" max="6" width="9" style="17"/>
+    <col min="7" max="7" width="49.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+    <row r="1" spans="1:7">
+      <c r="A1" s="18"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="18"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.6" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="8">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="5">
         <v>41900</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="8">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A6" s="18"/>
+      <c r="B6" s="5">
         <v>41892</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>0.125</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="8">
+    <row r="7" spans="1:7" ht="31.15" customHeight="1">
+      <c r="A7" s="18"/>
+      <c r="B7" s="5">
         <v>41907</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>0.125</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="21">
         <v>0.27083333333333298</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="8">
+    <row r="8" spans="1:7" ht="29.45" customHeight="1">
+      <c r="A8" s="18"/>
+      <c r="B8" s="5">
         <v>41939</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>0.16666666666666699</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0.14583333333333301</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="8">
+    <row r="9" spans="1:7" ht="28.15" customHeight="1">
+      <c r="A9" s="18"/>
+      <c r="B9" s="5">
         <v>41940</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>0.125</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="21">
         <v>0.140972222222222</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="8">
+    <row r="10" spans="1:7" ht="31.9" customHeight="1">
+      <c r="A10" s="18"/>
+      <c r="B10" s="5">
         <v>41941</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <v>9.8611111111111094E-2</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="8">
+    <row r="11" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A11" s="18"/>
+      <c r="B11" s="5">
         <v>41942</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>0.125</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="23">
         <v>0.16736111111111099</v>
       </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="8">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A12" s="18"/>
+      <c r="B12" s="5">
         <v>41943</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="23">
         <v>0.19861111111111099</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:7" ht="15" customHeight="1">
+      <c r="A13" s="18"/>
+      <c r="B13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="15">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="12">
         <f>SUM(E5:E12)</f>
         <v>0.85416666666666685</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <f>SUM(F5:F12)</f>
         <v>1.1263888888888878</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1610,252 +1811,252 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.140625"/>
-    <col min="3" max="3" width="15.5703125" style="4"/>
-    <col min="4" max="4" width="37.7109375" style="4"/>
-    <col min="5" max="5" width="14.85546875" style="20"/>
-    <col min="6" max="6" width="9.140625" style="20"/>
+    <col min="3" max="3" width="15.5703125" style="1"/>
+    <col min="4" max="4" width="37.7109375" style="1"/>
+    <col min="5" max="5" width="14.85546875" style="17"/>
+    <col min="6" max="6" width="9.140625" style="17"/>
     <col min="7" max="7" width="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="18"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="7" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="18"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="8">
+    <row r="5" spans="1:7">
+      <c r="A5" s="18"/>
+      <c r="B5" s="5">
         <v>41900</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="8">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="45">
+      <c r="A6" s="18"/>
+      <c r="B6" s="5">
         <v>41907</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>0.16666666666666699</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>0.16666666666666699</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="8">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" ht="30">
+      <c r="A7" s="18"/>
+      <c r="B7" s="5">
         <v>41914</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>0.125</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>0.27083333333333298</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="8">
+    <row r="8" spans="1:7">
+      <c r="A8" s="18"/>
+      <c r="B8" s="5">
         <v>41939</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>0.20833333333333301</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0.16666666666666699</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="8">
+    <row r="9" spans="1:7">
+      <c r="A9" s="18"/>
+      <c r="B9" s="5">
         <v>41940</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>0.16666666666666699</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="21">
         <v>0.140972222222222</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="8">
+    <row r="10" spans="1:7">
+      <c r="A10" s="18"/>
+      <c r="B10" s="5">
         <v>41941</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <v>9.8611111111111094E-2</v>
       </c>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="8">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="30">
+      <c r="A11" s="18"/>
+      <c r="B11" s="5">
         <v>41942</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="22">
         <v>0.125</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="21">
         <v>0.211111111111111</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="8">
+    <row r="12" spans="1:7">
+      <c r="A12" s="18"/>
+      <c r="B12" s="5">
         <v>41943</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="21">
         <v>0.20138888888888901</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:7" ht="15" customHeight="1">
+      <c r="A13" s="18"/>
+      <c r="B13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="15">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="12">
         <f>SUM(E5:E12)</f>
         <v>0.97916666666666674</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <f>SUM(F5:F12)</f>
         <v>1.2770833333333333</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1868,17 +2069,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
@@ -1888,266 +2089,266 @@
     <col min="7" max="7" width="37.7109375"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:7" ht="18.75" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="2:7" ht="14.45" customHeight="1">
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+    <row r="5" spans="2:7" ht="14.45" customHeight="1">
+      <c r="B5" s="5">
         <v>41900</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="32">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="32">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="32">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="34">
         <v>6.25E-2</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" ht="16.5" customHeight="1">
+      <c r="B7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="35">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="36">
         <v>0.14930555555555555</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" ht="30">
+      <c r="B8" s="5">
         <v>41914</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="35">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="35">
         <v>0.18055555555555555</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" ht="45.75" customHeight="1">
+      <c r="B9" s="5">
         <v>41708</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="36">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="35">
         <v>0.125</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
+    <row r="10" spans="2:7" ht="15" customHeight="1">
+      <c r="B10" s="5">
         <v>41921</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="35">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="36">
         <v>0.125</v>
       </c>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7" ht="31.5" customHeight="1">
+      <c r="B11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="35">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="36">
         <v>5.9027777777777783E-2</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="2:7" ht="45.75" customHeight="1">
+      <c r="B12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="35">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="36">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1">
+      <c r="B13" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="35">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="36">
         <v>0.20833333333333334</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="2:7" ht="31.5" customHeight="1">
+      <c r="B14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="35">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="36">
         <v>0.25</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="2:7" ht="31.5" customHeight="1">
+      <c r="B15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="35">
         <v>0.125</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="36">
         <v>0.21875</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+    <row r="16" spans="2:7">
+      <c r="B16" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="37">
         <f>SUM(E5:E15)</f>
         <v>0.78125</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="37">
         <f>SUM(F5:F15)</f>
         <v>1.4409722222222223</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2160,126 +2361,126 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" style="4"/>
-    <col min="3" max="3" width="14.28515625" style="4"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
+    <col min="2" max="2" width="10.5703125" style="1"/>
+    <col min="3" max="3" width="14.28515625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:4" ht="18.75">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+    <row r="5" spans="1:4">
+      <c r="B5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:4">
+      <c r="B6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="28">
         <f>SumEstBergler</f>
         <v>0.77083333333333315</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="28">
         <f>SumActBergler</f>
         <v>0.83414351851851909</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="1:4">
+      <c r="B7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="28">
         <f>SumEstBobek</f>
-        <v>2.0833333333333301E-2</v>
-      </c>
-      <c r="D7" s="31">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D7" s="28">
         <f>SumActBobek</f>
-        <v>2.0833333333333301E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="21">
         <f>SumEstJaneczek</f>
         <v>0.85416666666666685</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <f>SumActJaneczek</f>
         <v>1.1263888888888878</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+    <row r="9" spans="1:4">
+      <c r="B9" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="21">
         <f>SumEstMair</f>
         <v>0.97916666666666674</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <f>SumActMair</f>
         <v>1.2770833333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+    <row r="10" spans="1:4">
+      <c r="B10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="34">
         <v>0.78125</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="32">
         <v>1.4409722222222223</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="1:4">
+      <c r="B11" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="21">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
         <v>1.8333333333333335</v>
       </c>
-      <c r="D11" s="25">
-        <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>2.4034722222222209</v>
+      <c r="D11" s="22">
+        <f>SUM(SumActJaneczek+SumActMair+SumActBergler+SumActBobek+SumActOezsoy)</f>
+        <v>3.9459490740740732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>